<commit_message>
processing fticrms data from TMP1
</commit_message>
<xml_diff>
--- a/sample lists/Myers-Pigg_TEMPEST_FT_samplelist_Sept2023.xlsx
+++ b/sample lists/Myers-Pigg_TEMPEST_FT_samplelist_Sept2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/tempest-system-level-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/GitHub/TEMPEST-1-porewater/sample lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79E10326-264A-7042-912A-3E9D2A2C14E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FE7953-B0E9-E04B-8E86-2E30C7AB8B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{CACD97ED-0B41-CE43-B194-74CFD0BE7587}"/>
+    <workbookView xWindow="2060" yWindow="760" windowWidth="28160" windowHeight="19920" xr2:uid="{CACD97ED-0B41-CE43-B194-74CFD0BE7587}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>TMP_Methanol_Blk2</t>
   </si>
@@ -529,9 +529,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -569,7 +569,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -675,7 +675,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -817,7 +817,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -825,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7E9EF0-3331-EF4E-B93B-5AED3F256982}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B65"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,170 +1190,162 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>40</v>
+      <c r="A45" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>29</v>
+      <c r="A51" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>27</v>
+      <c r="A52" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>